<commit_message>
Se cambia la columna Incluido por una columna Excluido. Se han repasado las pruebas de aceptación y cambiado las unitarias y se adapta sin problema.
</commit_message>
<xml_diff>
--- a/EjerciciosLog/PrezConfig1.xlsx
+++ b/EjerciciosLog/PrezConfig1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sal8b\OneDrive\Escritorio\LibreriaMoodleAnalisis\EjerciciosLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D014E3DD-C389-4D27-A0E3-576220DCDCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BA3B2A-C172-47CB-A8E5-89690FF61BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Nombre completo del usuario</t>
   </si>
   <si>
-    <t>Incluido</t>
+    <t>Excluido</t>
+  </si>
+  <si>
+    <t>CASTILLO ROMERO, LÍA</t>
+  </si>
+  <si>
+    <t>CIDÓN HOFFMAN, JAIME</t>
+  </si>
+  <si>
+    <t>CIMAS CAMPOS, NOIVE</t>
+  </si>
+  <si>
+    <t>CUADRIELLO GALDÓS, ÁNGELA</t>
+  </si>
+  <si>
+    <t>CUEVAS RODRIGUEZ, SARA</t>
+  </si>
+  <si>
+    <t>DE SANTIAGO ABASCAL, GABRIELA</t>
+  </si>
+  <si>
+    <t>DE SÁDABA IGAREDA, CELIA</t>
+  </si>
+  <si>
+    <t>GUTIERREZ GUTIERREZ, MARTA</t>
+  </si>
+  <si>
+    <t>MUÑOZ GARCÍA, JAIME</t>
   </si>
   <si>
     <t>Pérez González, Docente</t>
   </si>
   <si>
-    <t>X</t>
+    <t>REVUELTA DIAZ, CRISTINA</t>
+  </si>
+  <si>
+    <t>RUIZ CORTÉS, CARLOTA</t>
+  </si>
+  <si>
+    <t>SAL SARRIA, SAÚL</t>
   </si>
   <si>
     <t>Contexto del evento</t>
@@ -42,42 +75,6 @@
   </si>
   <si>
     <t>Curso: G000 - Curso de Testing - Curso 2018-2019</t>
-  </si>
-  <si>
-    <t>CUADRIELLO GALDÓS, ÁNGELA</t>
-  </si>
-  <si>
-    <t>CUEVAS RODRIGUEZ, SARA</t>
-  </si>
-  <si>
-    <t>GUTIERREZ GUTIERREZ, MARTA</t>
-  </si>
-  <si>
-    <t>DE SÁDABA IGAREDA, CELIA</t>
-  </si>
-  <si>
-    <t>SAL SARRIA, SAÚL</t>
-  </si>
-  <si>
-    <t>DE SANTIAGO ABASCAL, GABRIELA</t>
-  </si>
-  <si>
-    <t>CIDÓN HOFFMAN, JAIME</t>
-  </si>
-  <si>
-    <t>RUIZ CORTÉS, CARLOTA</t>
-  </si>
-  <si>
-    <t>CIMAS CAMPOS, NOIVE</t>
-  </si>
-  <si>
-    <t>CASTILLO ROMERO, LÍA</t>
-  </si>
-  <si>
-    <t>MUÑOZ GARCÍA, JAIME</t>
-  </si>
-  <si>
-    <t>REVUELTA DIAZ, CRISTINA</t>
   </si>
 </sst>
 </file>
@@ -442,9 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -458,106 +453,67 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -569,24 +525,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="A3:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>